<commit_message>
Minor Friday updates, some graphs and README cleanup
</commit_message>
<xml_diff>
--- a/fitted_model_params_metrics.xlsx
+++ b/fitted_model_params_metrics.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owner/WORKING_FILES/GEN_ASSEMBLY/sandbox/mk_capstone/fitted_models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owner/WORKING_FILES/GEN_ASSEMBLY/sandbox/mk_capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C960730C-53E9-7F4D-BBF9-FFC12C208BF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2778628-1D15-8449-BC3A-D8CE6B90E225}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1560" windowWidth="25120" windowHeight="26600" xr2:uid="{746F708D-7A11-8E48-AB4D-9DBCF096E75E}"/>
+    <workbookView xWindow="1440" yWindow="1560" windowWidth="25120" windowHeight="26600" activeTab="1" xr2:uid="{746F708D-7A11-8E48-AB4D-9DBCF096E75E}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
-    <sheet name="ARIMA dam" sheetId="1" r:id="rId2"/>
-    <sheet name="ARIMA hasp" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="ARIMA dam" sheetId="1" r:id="rId3"/>
+    <sheet name="ARIMA hasp" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
   <si>
     <t>MODEL</t>
   </si>
@@ -144,6 +145,246 @@
   </si>
   <si>
     <t>Learn Rate</t>
+  </si>
+  <si>
+    <t>dam_price_per_mwh</t>
+  </si>
+  <si>
+    <t>hasp_price_per_mwh</t>
+  </si>
+  <si>
+    <t>rtm_price_per_mwh</t>
+  </si>
+  <si>
+    <t>7da_load_fcast_mw</t>
+  </si>
+  <si>
+    <t>2da_load_fcast_mw</t>
+  </si>
+  <si>
+    <t>dam_load_fcast_mw</t>
+  </si>
+  <si>
+    <t>rtm_load_fcast_mw</t>
+  </si>
+  <si>
+    <t>water_acre_feet</t>
+  </si>
+  <si>
+    <t>sand_temp</t>
+  </si>
+  <si>
+    <t>sand_wind</t>
+  </si>
+  <si>
+    <t>sand_vis</t>
+  </si>
+  <si>
+    <t>sand_ceil</t>
+  </si>
+  <si>
+    <t>fres_temp</t>
+  </si>
+  <si>
+    <t>fres_wind</t>
+  </si>
+  <si>
+    <t>fres_vis</t>
+  </si>
+  <si>
+    <t>fres_ceil</t>
+  </si>
+  <si>
+    <t>rive_temp</t>
+  </si>
+  <si>
+    <t>rive_wind</t>
+  </si>
+  <si>
+    <t>rive_vis</t>
+  </si>
+  <si>
+    <t>rive_ceil</t>
+  </si>
+  <si>
+    <t>redd_temp</t>
+  </si>
+  <si>
+    <t>redd_wind</t>
+  </si>
+  <si>
+    <t>redd_vis</t>
+  </si>
+  <si>
+    <t>redd_ceil</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>DATA DICTIONARY</t>
+  </si>
+  <si>
+    <t>ITEM NAME</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Datetime in Pacific time zone</t>
+  </si>
+  <si>
+    <t>Starts at 1:00am 01-01-2016, ending at 23:00 04-24-2019 with some gaps, for a total 29,067 rows</t>
+  </si>
+  <si>
+    <t>Train set</t>
+  </si>
+  <si>
+    <t>First 75% of data</t>
+  </si>
+  <si>
+    <t>21,800 rows</t>
+  </si>
+  <si>
+    <t>Test set</t>
+  </si>
+  <si>
+    <t>Last 25% of data</t>
+  </si>
+  <si>
+    <t>7,267 rows</t>
+  </si>
+  <si>
+    <t>Day Ahead Mkt electricity price (hourly)</t>
+  </si>
+  <si>
+    <t>DAM LMP (locational marginal price), In MWh (1 of 2 targets) at Bayshore SF node</t>
+  </si>
+  <si>
+    <t>Hour Ahead Sched Process price (15 min)</t>
+  </si>
+  <si>
+    <t>HASP LMP (locational marginal price, in MWh (2 of 2 targets), 15 min interval data down-sampled to hourly, at Bayshore SF node</t>
+  </si>
+  <si>
+    <t>Realtime spot price (5 min)</t>
+  </si>
+  <si>
+    <t>In MWh, 5 min interval data down-sampled to hourly, at Bayshore SF node</t>
+  </si>
+  <si>
+    <t>7 day load fcast</t>
+  </si>
+  <si>
+    <t>In MW, CA elec demand fcast, rolling 7 days in advance</t>
+  </si>
+  <si>
+    <t>2 day load fcast</t>
+  </si>
+  <si>
+    <t>In MW, CA elec demand fcast, rolling 2 days in advance</t>
+  </si>
+  <si>
+    <t>Day ahead load fcast</t>
+  </si>
+  <si>
+    <t>In MW, CA elec demand fcast, rolling one day in advance</t>
+  </si>
+  <si>
+    <t>Hour ahead load fcast</t>
+  </si>
+  <si>
+    <t>In MW, CA elec demand fcast, realtime, 1 hr in advance</t>
+  </si>
+  <si>
+    <t>CA Water Level</t>
+  </si>
+  <si>
+    <t>Total of 47 CA reservoirs' water content, in acre-feet</t>
+  </si>
+  <si>
+    <t>San Diego weather stn Temp</t>
+  </si>
+  <si>
+    <t>NOAA hrly data (-0932 to +0618) in deg C, scaling factor 10, NaN=9999</t>
+  </si>
+  <si>
+    <t>San Diego weather stn Sind speed</t>
+  </si>
+  <si>
+    <t>NOAA hrly data (0-900) in m/s, scaling factor 10, NaN=9999</t>
+  </si>
+  <si>
+    <t>San Diego weather stn Visibility</t>
+  </si>
+  <si>
+    <t>NOAA hrly data; horiz. visibility dist (0-160000 in m, scaling factor 1, NaN=999999</t>
+  </si>
+  <si>
+    <t>San Diego weather stn Ceiling</t>
+  </si>
+  <si>
+    <t>NOAA hrly data; cloud ceiling height (0-22000) in m, scaling factor 1, NaN=99999</t>
+  </si>
+  <si>
+    <t>Riverside weather stn Temp</t>
+  </si>
+  <si>
+    <t>Riverside weather stn Sind speed</t>
+  </si>
+  <si>
+    <t>Riverside weather stn Visibility</t>
+  </si>
+  <si>
+    <t>Riverside weather stn Ceiling</t>
+  </si>
+  <si>
+    <t>Redding weather stn Temp</t>
+  </si>
+  <si>
+    <t>Redding weather stn Sind speed</t>
+  </si>
+  <si>
+    <t>Redding weather stn Visibility</t>
+  </si>
+  <si>
+    <t>Redding weather stn Ceiling</t>
+  </si>
+  <si>
+    <t>Fresno weather stn Temp</t>
+  </si>
+  <si>
+    <t>Fresno weather stn Sind speed</t>
+  </si>
+  <si>
+    <t>Fresno weather stn Visibility</t>
+  </si>
+  <si>
+    <t>Fresno weather stn Ceiling</t>
+  </si>
+  <si>
+    <t>2016, 2017, 2018, 2019</t>
+  </si>
+  <si>
+    <t>0 - 23</t>
   </si>
 </sst>
 </file>
@@ -246,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -301,11 +542,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -522,6 +774,24 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -839,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60880E4-6528-9049-99F5-A322080B3A53}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.75" defaultRowHeight="15" customHeight="1"/>
@@ -995,19 +1265,26 @@
       <c r="L8" s="56"/>
       <c r="M8" s="56"/>
       <c r="N8" s="57">
-        <v>106.84</v>
+        <v>101.24</v>
       </c>
       <c r="O8" s="57">
-        <f t="shared" ref="O8:O9" si="0">N8^0.5</f>
-        <v>10.33634364753804</v>
+        <f t="shared" ref="O8" si="0">N8^0.5</f>
+        <v>10.061808982484212</v>
       </c>
       <c r="P8" s="56">
-        <v>0.74939999999999996</v>
+        <v>0.76249999999999996</v>
       </c>
       <c r="Q8" s="56"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="56"/>
+      <c r="R8" s="57">
+        <v>1692.87</v>
+      </c>
+      <c r="S8" s="57">
+        <f t="shared" ref="S8:S9" si="1">R8^0.5</f>
+        <v>41.144501455237005</v>
+      </c>
+      <c r="T8" s="56">
+        <v>-0.17319999999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:20" ht="15" customHeight="1">
       <c r="A9" s="64" t="s">
@@ -1034,19 +1311,25 @@
       <c r="L9" s="65"/>
       <c r="M9" s="65"/>
       <c r="N9" s="66">
-        <v>1009.8</v>
+        <v>991.07</v>
       </c>
       <c r="O9" s="66">
-        <f t="shared" si="0"/>
-        <v>31.777350424476865</v>
+        <f t="shared" ref="O8:O9" si="2">N9^0.5</f>
+        <v>31.481264269403159</v>
       </c>
       <c r="P9" s="65">
-        <v>0.39800000000000002</v>
+        <v>0.40920000000000001</v>
       </c>
       <c r="Q9" s="65"/>
-      <c r="R9" s="66"/>
-      <c r="S9" s="66"/>
-      <c r="T9" s="65"/>
+      <c r="R9" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="S9" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="T9" s="65">
+        <v>-0.1333</v>
+      </c>
     </row>
     <row r="10" spans="1:20" s="52" customFormat="1" ht="15" customHeight="1">
       <c r="C10" s="53"/>
@@ -1158,7 +1441,7 @@
         <v>105.45</v>
       </c>
       <c r="O13" s="63">
-        <f t="shared" ref="O13:O14" si="1">N13^0.5</f>
+        <f t="shared" ref="O13:O14" si="3">N13^0.5</f>
         <v>10.268885041717041</v>
       </c>
       <c r="P13" s="62">
@@ -1205,7 +1488,7 @@
         <v>1497.9</v>
       </c>
       <c r="O14" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>38.702713083193537</v>
       </c>
       <c r="P14" s="65">
@@ -1326,7 +1609,7 @@
         <v>127.6876</v>
       </c>
       <c r="O18" s="63">
-        <f t="shared" ref="O18:O20" si="2">N18^0.5</f>
+        <f t="shared" ref="O18:O20" si="4">N18^0.5</f>
         <v>11.299893804810734</v>
       </c>
       <c r="P18" s="62">
@@ -1337,7 +1620,7 @@
         <v>792.62139999999999</v>
       </c>
       <c r="S18" s="63">
-        <f t="shared" ref="S18:S20" si="3">R18^0.5</f>
+        <f t="shared" ref="S18:S20" si="5">R18^0.5</f>
         <v>28.15353263801898</v>
       </c>
       <c r="T18" s="62">
@@ -1384,7 +1667,7 @@
         <v>174.5455</v>
       </c>
       <c r="O19" s="66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.211566901772098</v>
       </c>
       <c r="P19" s="65">
@@ -1395,7 +1678,7 @@
         <v>816.26739999999995</v>
       </c>
       <c r="S19" s="66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28.570393766974931</v>
       </c>
       <c r="T19" s="65">
@@ -1442,7 +1725,7 @@
         <v>57.405099999999997</v>
       </c>
       <c r="O20" s="66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.5766153393187379</v>
       </c>
       <c r="P20" s="65">
@@ -1453,7 +1736,7 @@
         <v>762.8809</v>
       </c>
       <c r="S20" s="66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>27.62029869498156</v>
       </c>
       <c r="T20" s="65">
@@ -1520,7 +1803,7 @@
         <v>1386.8152</v>
       </c>
       <c r="O22" s="63">
-        <f t="shared" ref="O22:O24" si="4">N22^0.5</f>
+        <f t="shared" ref="O22:O24" si="6">N22^0.5</f>
         <v>37.239967776570374</v>
       </c>
       <c r="P22" s="62">
@@ -1531,7 +1814,7 @@
         <v>739.93100000000004</v>
       </c>
       <c r="S22" s="63">
-        <f t="shared" ref="S22:S24" si="5">R22^0.5</f>
+        <f t="shared" ref="S22:S24" si="7">R22^0.5</f>
         <v>27.201672742682572</v>
       </c>
       <c r="T22" s="62">
@@ -1578,7 +1861,7 @@
         <v>1378.7881</v>
       </c>
       <c r="O23" s="66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37.132036033592343</v>
       </c>
       <c r="P23" s="65">
@@ -1589,7 +1872,7 @@
         <v>777.17370000000005</v>
       </c>
       <c r="S23" s="66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>27.877835281814836</v>
       </c>
       <c r="T23" s="65">
@@ -1636,7 +1919,7 @@
         <v>790.92719999999997</v>
       </c>
       <c r="O24" s="66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>28.123427956065385</v>
       </c>
       <c r="P24" s="65">
@@ -1647,7 +1930,7 @@
         <v>843.16250000000002</v>
       </c>
       <c r="S24" s="66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>29.03726054571953</v>
       </c>
       <c r="T24" s="65">
@@ -1702,6 +1985,386 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334EB22F-9E35-F243-A8DA-102CFED698DA}">
+  <dimension ref="B3:D46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
+  <cols>
+    <col min="1" max="1" width="10.75" style="73"/>
+    <col min="2" max="2" width="18.75" style="73" customWidth="1"/>
+    <col min="3" max="3" width="28.75" style="73" customWidth="1"/>
+    <col min="4" max="4" width="66.75" style="73" customWidth="1"/>
+    <col min="5" max="16384" width="10.75" style="73"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" ht="12">
+      <c r="B3" s="73" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="12">
+      <c r="B5" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" s="74" customFormat="1" ht="24" customHeight="1">
+      <c r="B7" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B8" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B9" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="76" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1"/>
+    <row r="11" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B11" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B12" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1"/>
+    <row r="14" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B14" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="74" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1"/>
+    <row r="16" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B16" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="75" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B17" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="76" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B18" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="76" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B19" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="76" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1"/>
+    <row r="21" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B21" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="75" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="75" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1"/>
+    <row r="23" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B23" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B24" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B25" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="76" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B26" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="76" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1"/>
+    <row r="28" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B28" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B29" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B30" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="76" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B31" s="76" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="76" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1"/>
+    <row r="33" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B33" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B34" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B35" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="76" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B36" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="76" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1"/>
+    <row r="38" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B38" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B39" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="76" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" s="76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B40" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="76" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="76" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B41" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="76" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="76" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1"/>
+    <row r="43" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B43" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="75"/>
+    </row>
+    <row r="44" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B44" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="77">
+        <v>43477</v>
+      </c>
+      <c r="D44" s="76"/>
+    </row>
+    <row r="45" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B45" s="76" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="77">
+        <v>43496</v>
+      </c>
+      <c r="D45" s="76"/>
+    </row>
+    <row r="46" spans="2:4" s="74" customFormat="1" ht="12" customHeight="1">
+      <c r="B46" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="76"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BCD1E4-5EA4-B24B-9CE8-626E277C66C4}">
   <dimension ref="A1:R52"/>
   <sheetViews>
@@ -3216,7 +3879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5983817-A43E-2D4B-916C-0CE4D9C10DAB}">
   <dimension ref="A1:R57"/>
   <sheetViews>

</xml_diff>